<commit_message>
updated gantt chart week nov 21
</commit_message>
<xml_diff>
--- a/Gantt Chart Rosen A.xlsx
+++ b/Gantt Chart Rosen A.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BE69C9-0ABA-44C1-B053-4075DAB0649B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3131A7AA-9E66-4EEC-AEBF-063570AB4D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>Task 3</t>
   </si>
@@ -194,10 +194,31 @@
     <t>Reading Break</t>
   </si>
   <si>
-    <t>Started Developing Front-end, and VGG16 and Database Exploration</t>
-  </si>
-  <si>
-    <t>Login page, Fine-tune index and image html, keep working on database</t>
+    <t>1) Orvin 
+2) Ryan
+3) Fareeha
+4) Qingyan</t>
+  </si>
+  <si>
+    <t>1) Functionality of login 
+2) Functionality in index.html                                                                           
+3) Functionality image labeling 
+4) Database (continuation)</t>
+  </si>
+  <si>
+    <t>1) Orvin, Ryan
+2) Fareeha
+3) Qingyan</t>
+  </si>
+  <si>
+    <t>1) Started Developing Front-end
+2) Trying out VGG16  
+3) Database Exploration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Login page
+2) Fine-tune index.html                                                                           3) Fine tune image html 
+4) Exploration on vector database - Milvus </t>
   </si>
 </sst>
 </file>
@@ -603,7 +624,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -819,6 +840,15 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -831,26 +861,20 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1365,8 +1389,8 @@
   <dimension ref="A1:BL36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="96" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1409,106 +1433,106 @@
         <v>26</v>
       </c>
       <c r="B3" s="54"/>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="80">
+      <c r="D3" s="88"/>
+      <c r="E3" s="83">
         <v>44828</v>
       </c>
-      <c r="F3" s="80"/>
+      <c r="F3" s="83"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="82"/>
+      <c r="D4" s="88"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="77">
+      <c r="I4" s="80">
         <f>I5</f>
         <v>44823</v>
       </c>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="77">
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="80">
         <f>P5</f>
         <v>44830</v>
       </c>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="78"/>
-      <c r="S4" s="78"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="77">
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="82"/>
+      <c r="W4" s="80">
         <f>W5</f>
         <v>44837</v>
       </c>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="78"/>
-      <c r="AA4" s="78"/>
-      <c r="AB4" s="78"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="77">
+      <c r="X4" s="81"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="81"/>
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="82"/>
+      <c r="AD4" s="80">
         <f>AD5</f>
         <v>44844</v>
       </c>
-      <c r="AE4" s="78"/>
-      <c r="AF4" s="78"/>
-      <c r="AG4" s="78"/>
-      <c r="AH4" s="78"/>
-      <c r="AI4" s="78"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="77">
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="81"/>
+      <c r="AG4" s="81"/>
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="82"/>
+      <c r="AK4" s="80">
         <f>AK5</f>
         <v>44851</v>
       </c>
-      <c r="AL4" s="78"/>
-      <c r="AM4" s="78"/>
-      <c r="AN4" s="78"/>
-      <c r="AO4" s="78"/>
-      <c r="AP4" s="78"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="77">
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="81"/>
+      <c r="AN4" s="81"/>
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="82"/>
+      <c r="AR4" s="80">
         <f>AR5</f>
         <v>44858</v>
       </c>
-      <c r="AS4" s="78"/>
-      <c r="AT4" s="78"/>
-      <c r="AU4" s="78"/>
-      <c r="AV4" s="78"/>
-      <c r="AW4" s="78"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="77">
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="81"/>
+      <c r="AU4" s="81"/>
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="82"/>
+      <c r="AY4" s="80">
         <f>AY5</f>
         <v>44865</v>
       </c>
-      <c r="AZ4" s="78"/>
-      <c r="BA4" s="78"/>
-      <c r="BB4" s="78"/>
-      <c r="BC4" s="78"/>
-      <c r="BD4" s="78"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="77">
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="81"/>
+      <c r="BB4" s="81"/>
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="82"/>
+      <c r="BF4" s="80">
         <f>BF5</f>
         <v>44872</v>
       </c>
-      <c r="BG4" s="78"/>
-      <c r="BH4" s="78"/>
-      <c r="BI4" s="78"/>
-      <c r="BJ4" s="78"/>
-      <c r="BK4" s="78"/>
-      <c r="BL4" s="79"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="81"/>
+      <c r="BI4" s="81"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="82"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="49" t="s">
@@ -2598,13 +2622,13 @@
       <c r="AT14" s="44"/>
       <c r="AU14" s="44"/>
       <c r="AV14" s="44"/>
-      <c r="AW14" s="85"/>
-      <c r="AX14" s="83"/>
-      <c r="AY14" s="83"/>
-      <c r="AZ14" s="83"/>
-      <c r="BA14" s="83"/>
-      <c r="BB14" s="83"/>
-      <c r="BC14" s="84"/>
+      <c r="AW14" s="84"/>
+      <c r="AX14" s="85"/>
+      <c r="AY14" s="85"/>
+      <c r="AZ14" s="85"/>
+      <c r="BA14" s="85"/>
+      <c r="BB14" s="85"/>
+      <c r="BC14" s="86"/>
       <c r="BD14" s="44"/>
       <c r="BE14" s="44"/>
       <c r="BF14" s="44"/>
@@ -2615,13 +2639,13 @@
       <c r="BK14" s="44"/>
       <c r="BL14" s="44"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:64" s="3" customFormat="1" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="49"/>
-      <c r="B15" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="63" t="s">
-        <v>34</v>
+      <c r="B15" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="79" t="s">
+        <v>42</v>
       </c>
       <c r="D15" s="27">
         <v>1</v>
@@ -2698,7 +2722,7 @@
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="48"/>
-      <c r="B16" s="87" t="s">
+      <c r="B16" s="78" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="63"/>
@@ -2775,16 +2799,16 @@
       <c r="BK16" s="44"/>
       <c r="BL16" s="44"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="44.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:64" s="3" customFormat="1" ht="72.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="48"/>
-      <c r="B17" s="86" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="63" t="s">
-        <v>34</v>
+      <c r="B17" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="79" t="s">
+        <v>40</v>
       </c>
       <c r="D17" s="27">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="E17" s="56">
         <f>F16+1</f>
@@ -2856,13 +2880,17 @@
       <c r="BK17" s="44"/>
       <c r="BL17" s="44"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="63.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="48"/>
-      <c r="B18" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="63"/>
-      <c r="D18" s="27"/>
+      <c r="B18" s="77" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="79" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="27">
+        <v>0.25</v>
+      </c>
       <c r="E18" s="56">
         <f>F17+1</f>
         <v>44884</v>

</xml_diff>